<commit_message>
Added a cable based CNC machine link
</commit_message>
<xml_diff>
--- a/Research/Cord Based Systems Research.xlsx
+++ b/Research/Cord Based Systems Research.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t># words</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Muscle</t>
+  </si>
+  <si>
+    <t>2-axis CNC machine (akin to our robot)</t>
+  </si>
+  <si>
+    <t>https://youtu.be/05W4egqLVEM</t>
   </si>
 </sst>
 </file>
@@ -298,8 +304,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C27" totalsRowShown="0">
-  <autoFilter ref="A1:C27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C28" totalsRowShown="0">
+  <autoFilter ref="A1:C28"/>
   <tableColumns count="3">
     <tableColumn id="1" name="# words">
       <calculatedColumnFormula>IF(LEN(TRIM(B2))=0,0,LEN(TRIM(B2))-LEN(SUBSTITUTE(B2," ",""))+1)</calculatedColumnFormula>
@@ -823,10 +829,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,6 +1154,18 @@
       </c>
       <c r="C27" s="2" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>IF(LEN(TRIM(B28))=0,0,LEN(TRIM(B28))-LEN(SUBSTITUTE(B28," ",""))+1)</f>
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>